<commit_message>
Libero cobre del top abajo de los bnc Routeo reset cap Agrego componentes del reset a bom
</commit_message>
<xml_diff>
--- a/Bode_Analyzer/Bode_Analyzer.xlsx
+++ b/Bode_Analyzer/Bode_Analyzer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UTN\Nivel_4\Bode_Analyzer\Bode_Analyzer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A11EDE05-8B93-4715-8EA1-3B1548E6B06D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78EA9487-C90F-41EC-9E1A-D63629662876}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C29C70CA-A88C-40FF-93B4-D9D14F9D3D86}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="157">
   <si>
     <t>Comment</t>
   </si>
@@ -477,6 +477,39 @@
   </si>
   <si>
     <t>https://www.sycelectronica.com.ar/articulo.php?codigo=3296W-20K</t>
+  </si>
+  <si>
+    <t>2N7000_TO92</t>
+  </si>
+  <si>
+    <t>MOSFET N-CH 60V 200MA TO-92</t>
+  </si>
+  <si>
+    <t>TO92_DGS</t>
+  </si>
+  <si>
+    <t>MOSFET N</t>
+  </si>
+  <si>
+    <t>Q1, Q2</t>
+  </si>
+  <si>
+    <t>4K7</t>
+  </si>
+  <si>
+    <t>RES0805 4K7 5%</t>
+  </si>
+  <si>
+    <t>RES0805_4K7_5%</t>
+  </si>
+  <si>
+    <t>RMCF0805JT4K70TR-ND</t>
+  </si>
+  <si>
+    <t>RMCF0805JT4K70</t>
+  </si>
+  <si>
+    <t>R13, R14</t>
   </si>
 </sst>
 </file>
@@ -545,7 +578,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
@@ -555,8 +588,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -871,10 +902,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE21B3CF-F046-447C-8494-18DFB66E6CB5}">
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="A16:J16"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1112,56 +1143,56 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8" s="1">
         <v>1</v>
       </c>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="9" t="s">
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="J8" s="10"/>
+      <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F9" s="1">
         <v>1</v>
       </c>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="9" t="s">
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="J9" s="10"/>
+      <c r="J9" s="1"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
@@ -1626,6 +1657,62 @@
         <v>54</v>
       </c>
       <c r="J24" s="1"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="F25" s="2">
+        <v>2</v>
+      </c>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="F26" s="1">
+        <v>2</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>154</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Modifico resistencia de realimentacion de comparadores (cruce por cero a 100k), modifico descarga cap Vout a 220nF Arreglo PCB luego de hacer update Actualizo BOM
</commit_message>
<xml_diff>
--- a/Bode_Analyzer/Bode_Analyzer.xlsx
+++ b/Bode_Analyzer/Bode_Analyzer.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UTN\Nivel_4\Bode_Analyzer\Bode_Analyzer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78EA9487-C90F-41EC-9E1A-D63629662876}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6C0AD5C-C07E-432A-BB1F-3C6C8167BCF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C29C70CA-A88C-40FF-93B4-D9D14F9D3D86}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="154">
   <si>
     <t>Comment</t>
   </si>
@@ -137,9 +137,6 @@
     <t>CAP CER RAD 100NF 250V C0G 10%</t>
   </si>
   <si>
-    <t>C22, C23</t>
-  </si>
-  <si>
     <t>CAP508</t>
   </si>
   <si>
@@ -299,9 +296,6 @@
     <t>RES0805 100K 1%</t>
   </si>
   <si>
-    <t>R1, R7, R8</t>
-  </si>
-  <si>
     <t>RES0805_100K_1%</t>
   </si>
   <si>
@@ -374,24 +368,6 @@
     <t>3296W-104LF-ND</t>
   </si>
   <si>
-    <t>22K 1%</t>
-  </si>
-  <si>
-    <t>RES0805 22K 1%</t>
-  </si>
-  <si>
-    <t>R6, R11</t>
-  </si>
-  <si>
-    <t>RES0805_22K_1%</t>
-  </si>
-  <si>
-    <t>RMCF0805FT22K0</t>
-  </si>
-  <si>
-    <t>RMCF0805FT22K0CT-ND</t>
-  </si>
-  <si>
     <t>680R</t>
   </si>
   <si>
@@ -510,6 +486,21 @@
   </si>
   <si>
     <t>R13, R14</t>
+  </si>
+  <si>
+    <t>R1, R6, R7, R8, R11</t>
+  </si>
+  <si>
+    <t>220nF</t>
+  </si>
+  <si>
+    <t>CAP CER RAD 220NF 250V C0G 10%</t>
+  </si>
+  <si>
+    <t>C22</t>
+  </si>
+  <si>
+    <t>C23</t>
   </si>
 </sst>
 </file>
@@ -578,7 +569,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
@@ -588,6 +579,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -905,17 +899,21 @@
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="20" customWidth="1"/>
+    <col min="3" max="3" width="47.140625" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20" customWidth="1"/>
-    <col min="7" max="10" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -950,14 +948,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -1014,14 +1012,14 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="9" t="s">
         <v>26</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -1048,22 +1046,22 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>10</v>
+        <v>150</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>31</v>
+        <v>151</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="E5" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="F5" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>15</v>
@@ -1079,110 +1077,116 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F6" s="1">
-        <v>2</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="I6" s="2" t="s">
+      <c r="A6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="6">
+        <v>1</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J6" s="2" t="s">
-        <v>42</v>
+      <c r="J6" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="F7" s="1">
         <v>2</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>23</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="F8" s="1">
-        <v>1</v>
-      </c>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="I8" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="J8" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="F9" s="1">
         <v>1</v>
@@ -1190,405 +1194,399 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="B10" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="C11" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="D11" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F11" s="8">
+        <v>2</v>
+      </c>
+      <c r="G11" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="D10" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="F10" s="8">
-        <v>2</v>
-      </c>
-      <c r="G10" s="7" t="s">
+      <c r="H11" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="I11" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J11" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="I10" s="7" t="s">
+      <c r="K11" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="I12" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J10" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="K10" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F11" s="1">
+      <c r="J12" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="F13" s="6">
         <v>1</v>
       </c>
-      <c r="G11" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="I11" s="2" t="s">
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="F14" s="8">
+        <v>1</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="I14" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="J11" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="F12" s="6">
-        <v>1</v>
-      </c>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="F13" s="8">
-        <v>1</v>
-      </c>
-      <c r="G13" s="7" t="s">
+      <c r="J14" s="7" t="s">
         <v>82</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="J13" s="7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="F14" s="1">
-        <v>3</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>93</v>
+        <v>149</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="F15" s="1">
         <v>3</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>23</v>
       </c>
       <c r="J15" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F16" s="1">
+        <v>3</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
+      <c r="C17" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="D17" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="E17" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="F17" s="8">
+        <v>1</v>
+      </c>
+      <c r="G17" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="H17" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="F16" s="8">
+      <c r="I17" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="K17" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F18" s="1">
         <v>1</v>
       </c>
-      <c r="G16" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="I16" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="J16" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="K16" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C17" s="2" t="s">
+      <c r="G18" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H18" s="2" t="s">
         <v>107</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="F17" s="1">
-        <v>1</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="F18" s="1">
-        <v>2</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>115</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>23</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="F19" s="1">
         <v>2</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>23</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="F20" s="6">
         <v>1</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="I20" s="5" t="s">
         <v>23</v>
       </c>
       <c r="J20" s="6"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="F21" s="6">
         <v>4</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="I21" s="5" t="s">
         <v>23</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="F22" s="6">
         <v>4</v>
@@ -1603,24 +1601,24 @@
         <v>23</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="F23" s="1">
         <v>1</v>
@@ -1628,25 +1626,25 @@
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J23" s="1"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="F24" s="1">
         <v>1</v>
@@ -1654,25 +1652,25 @@
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J24" s="1"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="F25" s="2">
         <v>2</v>
@@ -1682,36 +1680,36 @@
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="F26" s="1">
         <v>2</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="I26" s="2" t="s">
         <v>23</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>